<commit_message>
Updated the data in Test.xlsx
</commit_message>
<xml_diff>
--- a/Test_Mobile_Andriod_demo_docker/src/test/java/test_data/Test.xlsx
+++ b/Test_Mobile_Andriod_demo_docker/src/test/java/test_data/Test.xlsx
@@ -1,27 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\318356\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A8BF62-59A8-4D68-84B8-F494904D52AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="3990" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="TestCase" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Result" sheetId="6" r:id="rId4"/>
+    <sheet name="PatientMetaData test" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A5:Q13"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="121">
   <si>
     <t>DOB</t>
   </si>
@@ -62,46 +78,100 @@
     <t>Jan 08 2002</t>
   </si>
   <si>
+    <t>Father_3</t>
+  </si>
+  <si>
+    <t>Mother_3</t>
+  </si>
+  <si>
     <t>Jan 08 2003</t>
   </si>
   <si>
-    <t>Father_3</t>
-  </si>
-  <si>
     <t>Father_4</t>
   </si>
   <si>
-    <t>Mother_3</t>
-  </si>
-  <si>
     <t>Mother_4</t>
   </si>
   <si>
     <t>Jan 08 2004</t>
   </si>
   <si>
+    <t>Father_5</t>
+  </si>
+  <si>
+    <t>Mother_6</t>
+  </si>
+  <si>
     <t>Jan 08 1986</t>
   </si>
   <si>
+    <t>Father_6</t>
+  </si>
+  <si>
+    <t>Mother_7</t>
+  </si>
+  <si>
     <t>Jan 08 1987</t>
   </si>
   <si>
-    <t>Father_5</t>
-  </si>
-  <si>
-    <t>Father_6</t>
-  </si>
-  <si>
     <t>Father_7</t>
   </si>
   <si>
     <t>Mother_8</t>
   </si>
   <si>
-    <t>Mother_7</t>
-  </si>
-  <si>
-    <t>Mother_6</t>
+    <t>Android Test Automation Protocol</t>
+  </si>
+  <si>
+    <t>Test case</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP_Home_Screen </t>
+  </si>
+  <si>
+    <t>DP_Home_Screen_TC_1</t>
+  </si>
+  <si>
+    <t>checking the "cancel" button in the pop-up window of the add patient button and thus by checking the "AddPatient button"</t>
+  </si>
+  <si>
+    <t>DP_Home_Screen_TC_2</t>
+  </si>
+  <si>
+    <t>checking the "ok" button in the pop-up window of the add patient button and thus by checking the "AddPatient button"</t>
+  </si>
+  <si>
+    <t>DP_Home_Screen_TC_3</t>
+  </si>
+  <si>
+    <t>checking the add patient screen</t>
+  </si>
+  <si>
+    <t>DP_Home_Screen_TC_4</t>
+  </si>
+  <si>
+    <t>checking the  patient meta data  screen</t>
+  </si>
+  <si>
+    <t>DP_Home_Screen_TC_5</t>
+  </si>
+  <si>
+    <t>checking the add appointment screen</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
   <si>
     <t>Mother_5</t>
@@ -113,17 +183,306 @@
     <t>Mother_9</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
+    <t>checking home screen  for the content verification</t>
+  </si>
+  <si>
+    <t>1. confirm the elements and its contents and its positions are present 
+2.  Verify the result.</t>
+  </si>
+  <si>
+    <t>1. Test scripts should verify the elements and contents matching with the contents and positions which is mentioned in the picture under Results tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The home screen shall be present
+2. The patient screen the shall be empty </t>
+  </si>
+  <si>
+    <t>DP_Home_Screen_TC_0</t>
+  </si>
+  <si>
+    <t>1.The Patient meta data screen shall contain the age,dob,gender,father's name and mother's name at the end of the data provider test case</t>
+  </si>
+  <si>
+    <t>1. The patient meta data screen shall be present as per the PatientMetaData test tab according to the patient name.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The corresponding patient meta data (Test Pateint1) screen shall be present
+2. The appointment screen shall be present with the corresponding patient . </t>
+  </si>
+  <si>
+    <t>Problem Faced</t>
+  </si>
+  <si>
+    <t>Fix done</t>
+  </si>
+  <si>
+    <t>Save button was showing the n such elementin the screen</t>
+  </si>
+  <si>
+    <t>In this case the problem was the android keyboard was pop up and hiding the save button, and thus it was throwing the error.
+As a fix the there was a2 ideas;
+1. Add a command in the set caability  (Not imlemented due to changes in jar file).
+2. Add driver.hidekeyboard();</t>
+  </si>
+  <si>
+    <t>1. Position checks of the elements
+2. checking the images are correct</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Popped up text selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The Patient meta data screen shall be present with the first and last name on it
+2. The patient screen the shall be filled with the first name and last name which is given in the step 3. </t>
+  </si>
+  <si>
+    <t>1. Navigate to home screen
+2. Click the "Add Patient button"
+3. Provide the first name, and last name.
+4. click the "cancel" button.
+5. Verify the result 1.
+6. Click the "patient" button.
+7. Verify the result 2.
+8. Delete the entry after the test case verification.</t>
+  </si>
+  <si>
+    <t>1. Navigate to home screen
+2. Click the Add patient in the home screen
+3. click the added patient in the add patient screen.
+4. Provide the DOB, gender, Father's Name, Mother's Name
+5. click the "ok" button.
+6. Verify the result.
+7. Delete the entry after the test case verification.</t>
+  </si>
+  <si>
+    <t>1. Navigate to home screen
+2. Click the "Add Patient button"
+3. Provide the first name, and last name
+4. click the "ok" button.
+5. Verify the result.
+6. Navigate to the home screen and the then to patien screen.
+7. Verify the result.
+8. Delete the entry after the test case verification.</t>
+  </si>
+  <si>
+    <t>1. Navigate to home screen
+2. Click the Add patient in the home screen
+3. Add new patient pop-up will present a
+4. Provide the first name, and last name using test scripts.
+5. click the "DONE" button.
+6. Patient metadata screen will be up, click the Base info in the patient tab, Enter the details such as DOB, Age, Gender, Father's Name , and Mother's name using the test scripts. 
+7. click the "SAVE" button.
+8.  Patient metadata screen will be up, click the Address  in the patient tab, Enter the details such as Address, phone , Alt phone and Email . 
+9. click the "SAVE" button.
+10.  Patient metadata screen will be up, click the Notes in the patient tab, Enter the details such as Blood Type, Weight, Height, Company and Occupation using the test scripts. 
+11. click the "SAVE" button.
+12. Get the scrren shot of the Patient tab.
+13.  Patient metadata screen will be up, click the Notes in the documents tab, Enter the details such as document notes.
+14. click the "SAVE" button.
+15. Get the scrren shot of the Patient tab.
+16. Verify the results.
+17. Delete the entry after the test case verification.
+Note: The negative test cases are also provided using data provider fuctionality as per PatientMetaData test tab</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Navigate to home screen.
+2. Click the add Appointment  in the home screen.
+3.New appointment screen will be up; click the visit date, and give the date and time.
+4. click the patient and tesxt box and select the already added patient (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test Pateint1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) .
+5. click on the Reason for visit and add the reason.
+6. Click the save button in the screen.
+7. Verify Result 1.
+8. Go to home screen and then to apointments select the date mentiond in the step 3.
+9.  Verify the Result 2.
+10. Delete the entry after the test case verification.</t>
+    </r>
+  </si>
+  <si>
+    <t>Home screen 3</t>
+  </si>
+  <si>
+    <t>Home screen 2</t>
+  </si>
+  <si>
+    <t>Home screen 1</t>
+  </si>
+  <si>
+    <t>Reference Image for Verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen Name </t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>O-</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Addr8</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Addr7</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Farmer</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>Test Addr6</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Jaison</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>Test Addr5</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>wron</t>
+  </si>
+  <si>
+    <t>test2@gmail</t>
+  </si>
+  <si>
+    <t>Test Addr4</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>Chemist</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Test Addr2</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Test Addr1</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Agnel</t>
+  </si>
+  <si>
+    <t>Com</t>
+  </si>
+  <si>
+    <t>Occu</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>APh</t>
+  </si>
+  <si>
+    <t>Ph</t>
+  </si>
+  <si>
+    <t>Addr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,16 +498,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -171,14 +543,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,6 +665,146 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2562225" cy="3600450"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C07B4325-BD97-4F74-B0E9-9BD7D8621ED1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="342900"/>
+          <a:ext cx="2562225" cy="3600450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2457449" cy="5127839"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95C61E9E-8B6A-46B1-B57D-F90DE0978C82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="390525"/>
+          <a:ext cx="2457449" cy="5127839"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1209676</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2314574" cy="4795239"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9D1910E-D4D9-4DE9-A81F-E306065C66AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828801" y="676276"/>
+          <a:ext cx="2314574" cy="4795239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,10 +1069,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -472,8 +1083,7 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +1097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -501,7 +1111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -515,7 +1125,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -523,27 +1133,27 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -551,15 +1161,15 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -568,34 +1178,224 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000Internal Use&amp;1#</oddHeader>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Internal Use</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000Internal Use&amp;1#</oddHeader>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Internal Use</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -606,7 +1406,7 @@
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,12 +1420,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -634,106 +1434,547 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000Internal Use&amp;1#</oddHeader>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Internal Use</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BD0637-9031-419D-B39C-1ECD995F8DA6}">
+  <dimension ref="B1:C4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="299.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="405" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="2:3" ht="405.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000Internal Use&amp;1#</oddHeader>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Internal Use</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C02FA-1523-422E-843D-D1192C08B191}">
+  <dimension ref="B1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="2">
+        <v>9874563210</v>
+      </c>
+      <c r="H2" s="2">
+        <v>887456321210</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="2">
+        <v>171</v>
+      </c>
+      <c r="L2" s="2">
+        <v>67</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9874560043211</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8874563211</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="2">
+        <v>172</v>
+      </c>
+      <c r="L3" s="2">
+        <v>65</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>8874563210</v>
+      </c>
+      <c r="H4" s="2">
+        <v>9874563211</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="2">
+        <v>173</v>
+      </c>
+      <c r="L4" s="2">
+        <v>639</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="2">
+        <v>8874563211</v>
+      </c>
+      <c r="H5" s="2">
+        <v>9874563210</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="2">
+        <v>174</v>
+      </c>
+      <c r="L5" s="2">
+        <v>71</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="2">
+        <v>8874563210</v>
+      </c>
+      <c r="H6" s="2">
+        <v>9874563210</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="2">
+        <v>15575</v>
+      </c>
+      <c r="L6" s="2">
+        <v>72</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8874563211</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9874563211</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="2">
+        <v>172</v>
+      </c>
+      <c r="L7" s="2">
+        <v>58</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="2">
+        <v>9874563211</v>
+      </c>
+      <c r="H8" s="2">
+        <v>8874563210</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" s="2">
+        <v>173</v>
+      </c>
+      <c r="L8" s="2">
+        <v>25</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="2">
+        <v>9874563210</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8874563211</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="2">
+        <v>174</v>
+      </c>
+      <c r="L9" s="2">
+        <v>55</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000Internal Use&amp;1#</oddHeader>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Internal Use</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>